<commit_message>
Cambios que no funcionaban en casa
</commit_message>
<xml_diff>
--- a/PruebasElisa/php/facturacion.xlsx
+++ b/PruebasElisa/php/facturacion.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Apache Software Foundation\Apache2.2\htdocs\proyecto\PruebasElisa\php\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$3</definedName>
-    <definedName name="datos" localSheetId="0">Hoja1!$A$2:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$5</definedName>
+    <definedName name="datos" localSheetId="0">Hoja1!$A$2:$J$5</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="datos" type="6" refreshedVersion="4" background="1" refreshOnLoad="1" saveData="1">
-    <textPr prompt="0" codePage="850" firstRow="2" sourceFile="C:\wamp\www\proyecto\PruebasElisa\php\datos.csv" decimal="," thousands="." comma="1">
-      <textFields count="11">
-        <textField/>
+  <connection id="1" name="datos" type="6" refreshedVersion="5" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="850" firstRow="2" sourceFile="http://localhost/proyecto/pruebasElisa/php/datos.csv" decimal="," thousands="." comma="1">
+      <textFields count="10">
         <textField/>
         <textField/>
         <textField/>
@@ -42,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Nombre</t>
   </si>
@@ -89,13 +96,13 @@
     <t xml:space="preserve"> Tarifa 1/s</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2015-04-11 19:24:29</t>
+    <t xml:space="preserve"> 2015-04-21 12:23:30</t>
   </si>
   <si>
     <t xml:space="preserve"> 0000-00-00 00:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve"> Domiciliacion</t>
+    <t xml:space="preserve"> SI</t>
   </si>
   <si>
     <t xml:space="preserve"> nose@asd.es </t>
@@ -110,7 +117,31 @@
     <t xml:space="preserve"> 2015-04-11 19:47:14</t>
   </si>
   <si>
+    <t xml:space="preserve"> NO</t>
+  </si>
+  <si>
     <t xml:space="preserve"> asd </t>
+  </si>
+  <si>
+    <t>Elisa Tarancon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2015-04-20 16:19:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> algo@algo.algo </t>
+  </si>
+  <si>
+    <t>ALguien Apellida Algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2015-04-20 16:26:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> some@thi.n </t>
   </si>
 </sst>
 </file>
@@ -168,17 +199,20 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="datos" refreshOnLoad="1" growShrinkType="overwriteClear" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="datos" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -192,39 +226,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,7 +293,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,188 +337,164 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -574,42 +584,81 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I3">
         <v>55555</v>
       </c>
       <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
+      </c>
+      <c r="I4">
+        <v>654654654</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <v>666555444</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H3"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <autoFilter ref="A1:H5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>